<commit_message>
Add URL column to resources spreadsheet
</commit_message>
<xml_diff>
--- a/assets/doc/DMU_Data_Dojo_-_Power_BI_Learning_Resources.xlsx
+++ b/assets/doc/DMU_Data_Dojo_-_Power_BI_Learning_Resources.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\GitHub\DataVolumeXYZ\assets\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbartlett\GitHub\DataVolumeXYZ\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B82235-7DD4-4CA7-B104-DE977980681A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742B2ECE-D06B-4224-B1E8-C49BE9CCD286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="2540" windowWidth="28620" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="2940" windowWidth="32580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power BI Learning Resources" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -25,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +37,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="51">
+  <si>
+    <t>Name</t>
+  </si>
   <si>
     <t>Recommended Order</t>
   </si>
@@ -115,6 +123,9 @@
     <t>Videoconference</t>
   </si>
   <si>
+    <t>Free Power BI "Paginated Reports in a Day" Self-Paced Course</t>
+  </si>
+  <si>
     <t>Use DAX in Power BI Desktop</t>
   </si>
   <si>
@@ -127,14 +138,65 @@
     <t>Administer Power BI, Part 2 - Premium, Power BI Embedded, Automation</t>
   </si>
   <si>
-    <t>Power BI Learning Resource</t>
+    <t>https://www.linkedin.com/learning/learning-data-visualization-3</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/learning/getting-started-with-power-bi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/learning/power-bi-essential-training-3</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/learning/learning-microsoft-power-bi-desktop-14165789</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/consume-data-with-power-bi/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/power-bi-effective/?source=learn</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/create-use-analytics-reports-power-bi/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/prepare-data-power-bi/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/model-power-bi/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/visualize-data-power-bi/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/perform-analytics-power-bi/</t>
+  </si>
+  <si>
+    <t>https://events.microsoft.com/en-us/allevents/?search=Dashboard%20in%20a%20Day&amp;language=English&amp;clientTimeZone=1&amp;startTime=07:30&amp;endTime=11:00</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/en-us/power-bi/learning-catalog/paginated-reports-online-course</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/dax-power-bi/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/manage-workspaces-datasets-power-bi/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/administer-power-bi-part-1/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/learn/paths/administer-power-bi-part-2/</t>
+  </si>
+  <si>
+    <t>URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,14 +208,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.14996795556505021"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,33 +234,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.14996795556505021"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -220,13 +256,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}" name="Table1" displayName="Table1" ref="A1:G17" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:G17" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
-    <sortCondition ref="B1:B17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}" name="Table1" displayName="Table1" ref="A1:H19" totalsRowShown="0">
+  <autoFilter ref="A1:H19" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H18">
+    <sortCondition ref="C1:C18"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1CEE721A-4406-4C48-BE58-BFD0E5ED15DB}" name="Power BI Learning Resource"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{1CEE721A-4406-4C48-BE58-BFD0E5ED15DB}" name="Name"/>
+    <tableColumn id="9" xr3:uid="{B18A3F2B-C1A7-4B99-9499-97868F59CAB0}" name="URL" dataCellStyle="Hyperlink"/>
     <tableColumn id="7" xr3:uid="{7F43309C-1EDD-4AEB-916F-408ADE52696B}" name="Recommended Order" dataCellStyle="Hyperlink"/>
     <tableColumn id="5" xr3:uid="{961526F8-3AD4-4E63-94CC-1878A9CBB30E}" name="Source" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{54078CC2-43A3-4099-95A1-31E1003D07A8}" name="Primary Content Type"/>
@@ -234,14 +271,14 @@
     <tableColumn id="3" xr3:uid="{B5D01D82-E5CE-4461-9A6B-C2074B025BB0}" name="Learning Level"/>
     <tableColumn id="4" xr3:uid="{15C22E76-B2B0-4B0D-983C-0B5693F54D5C}" name="Time Commitment (Hours)"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +316,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,58 +572,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="66.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" customWidth="1"/>
-    <col min="3" max="3" width="29.7265625" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" customWidth="1"/>
-    <col min="7" max="7" width="28.36328125" customWidth="1"/>
+    <col min="2" max="2" width="64.26953125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -597,19 +635,22 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -620,19 +661,22 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
         <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -643,19 +687,22 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4">
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
         <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -666,180 +713,204 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
         <v>2.75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12">
+      <c r="H12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13">
         <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -848,128 +919,175 @@
         <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15">
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15">
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16">
         <v>1.25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17">
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18">
         <v>1.25</v>
       </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A7" r:id="rId1" display="Design effective reports in Power BI - Learn | Microsoft Docs" xr:uid="{D6FD071E-86A2-4974-ACE4-F0D15784803C}"/>
-    <hyperlink ref="A14" r:id="rId2" display="Use DAX in Power BI Desktop - Learn | Microsoft Docs" xr:uid="{BA465A39-9E0B-4FFE-B1C0-68065ADF7AB9}"/>
+    <hyperlink ref="A15" r:id="rId2" display="Use DAX in Power BI Desktop - Learn | Microsoft Docs" xr:uid="{BA465A39-9E0B-4FFE-B1C0-68065ADF7AB9}"/>
     <hyperlink ref="A9" r:id="rId3" display="Prepare data for analysis - Learn | Microsoft Docs" xr:uid="{620B21B5-C330-4FC9-8F30-373F20BCEB8A}"/>
     <hyperlink ref="A10" r:id="rId4" display="Model data in Power BI - Learn | Microsoft Docs" xr:uid="{A0AB4F13-8BCE-4ABB-AEC5-7C673F95C2EB}"/>
     <hyperlink ref="A11" r:id="rId5" display="Visualize data in Power BI - Learn | Microsoft Docs" xr:uid="{0151A887-F397-4800-A86A-57282DECA371}"/>
     <hyperlink ref="A6" r:id="rId6" display="Consume data with Power BI - Learn | Microsoft Docs" xr:uid="{0D81DD45-94F1-4E60-A69C-BE47F4AB2D05}"/>
     <hyperlink ref="A8" r:id="rId7" display="Create and use analytics reports with Power BI - Learn | Microsoft Docs" xr:uid="{417B315C-D931-4262-B441-5979A1E17521}"/>
     <hyperlink ref="A12" r:id="rId8" display="Data analysis in Power BI - Learn | Microsoft Docs" xr:uid="{C1821313-DF30-470F-BD57-D2FF0B85C16B}"/>
-    <hyperlink ref="A16" r:id="rId9" display="Administer Power BI, Part 1 - Tenants, governance, collaboration - Learn | Microsoft Docs" xr:uid="{D6A9F8FA-1058-4D7E-96EF-63C4FA17BC26}"/>
-    <hyperlink ref="A17" r:id="rId10" display="Administer Power BI, Part 2 - Premium, Power BI embedded, automation - Learn | Microsoft Docs" xr:uid="{FC5DE8BE-061B-49B4-ADAE-96DBE72A7D36}"/>
-    <hyperlink ref="A15" r:id="rId11" display="Manage workspaces and datasets in Power BI - Learn | Microsoft Docs" xr:uid="{7110D2D5-A09D-45E6-98B5-A229513200FC}"/>
+    <hyperlink ref="A17" r:id="rId9" display="Administer Power BI, Part 1 - Tenants, governance, collaboration - Learn | Microsoft Docs" xr:uid="{D6A9F8FA-1058-4D7E-96EF-63C4FA17BC26}"/>
+    <hyperlink ref="A18" r:id="rId10" display="Administer Power BI, Part 2 - Premium, Power BI embedded, automation - Learn | Microsoft Docs" xr:uid="{FC5DE8BE-061B-49B4-ADAE-96DBE72A7D36}"/>
+    <hyperlink ref="A16" r:id="rId11" display="Manage workspaces and datasets in Power BI - Learn | Microsoft Docs" xr:uid="{7110D2D5-A09D-45E6-98B5-A229513200FC}"/>
     <hyperlink ref="A2" r:id="rId12" xr:uid="{4FBFE39A-D3FB-45AC-82F1-B5D54E01316B}"/>
     <hyperlink ref="A3" r:id="rId13" xr:uid="{95CF5DB6-FB08-4FA3-8BCF-426925A4FBBE}"/>
     <hyperlink ref="A4" r:id="rId14" xr:uid="{7FA9A9B5-006B-406F-8778-BF73160F113D}"/>
     <hyperlink ref="A5" r:id="rId15" xr:uid="{0AA3A633-97A7-437B-A9FB-74644C130B33}"/>
     <hyperlink ref="A13" r:id="rId16" xr:uid="{A576D028-DE37-4872-80DE-2DCADDB63D4F}"/>
+    <hyperlink ref="A14" r:id="rId17" display="Power BI Paginated Reports in a Day Self-Paced Course" xr:uid="{34A1C306-1953-4FFF-9573-2945D4BEB9FB}"/>
   </hyperlinks>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
-  <pageSetup scale="61" orientation="landscape" r:id="rId17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1002,8 +1120,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001D9FC6984F93BD419C7571DBF45988AB" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed5663b85015e6b9c5f9cf128629760d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1cecf776-dfdf-4719-9fbc-71803a404f26" xmlns:ns3="6ac90070-c7bb-46a5-80a9-4cc49ad71337" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ab0a557fff89614fdb225018d300d75" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001D9FC6984F93BD419C7571DBF45988AB" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c8c53b20fd05820e33b576693dd438d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1cecf776-dfdf-4719-9fbc-71803a404f26" xmlns:ns3="6ac90070-c7bb-46a5-80a9-4cc49ad71337" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bf54877d6e26342d29e1a0e89ce09566" ns2:_="" ns3:_="">
     <xsd:import namespace="1cecf776-dfdf-4719-9fbc-71803a404f26"/>
     <xsd:import namespace="6ac90070-c7bb-46a5-80a9-4cc49ad71337"/>
     <xsd:element name="properties">
@@ -1026,6 +1144,8 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1096,6 +1216,16 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6ac90070-c7bb-46a5-80a9-4cc49ad71337" elementFormDefault="qualified">
@@ -1241,10 +1371,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5C34FB-9508-4CCC-91FE-4064A913EE20}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1cecf776-dfdf-4719-9fbc-71803a404f26"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="6ac90070-c7bb-46a5-80a9-4cc49ad71337"/>
-    <ds:schemaRef ds:uri="1cecf776-dfdf-4719-9fbc-71803a404f26"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1258,7 +1394,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3561B59F-F7D8-4716-83BF-3DBA0EE8BC5D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15519C5-3262-4FBD-81E4-C4BA63CC4AB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>

<commit_message>
fixed table name, removed blank row
</commit_message>
<xml_diff>
--- a/assets/doc/DMU_Data_Dojo_-_Power_BI_Learning_Resources.xlsx
+++ b/assets/doc/DMU_Data_Dojo_-_Power_BI_Learning_Resources.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbartlett\GitHub\DataVolumeXYZ\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742B2ECE-D06B-4224-B1E8-C49BE9CCD286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E418B7E-621A-4A6A-93C3-A419A943D6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="2940" windowWidth="32580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="2270" windowWidth="32580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power BI Learning Resources" sheetId="1" r:id="rId1"/>
@@ -256,8 +256,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}" name="Table1" displayName="Table1" ref="A1:H19" totalsRowShown="0">
-  <autoFilter ref="A1:H19" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}" name="Power_BI_Learning_Resources" displayName="Power_BI_Learning_Resources" ref="A1:H18" totalsRowShown="0">
+  <autoFilter ref="A1:H18" xr:uid="{C8B7E594-DE05-4375-A97C-AFC2C6F2A1B3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H18">
     <sortCondition ref="C1:C18"/>
   </sortState>
@@ -572,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,12 +1057,6 @@
       <c r="H18">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1093,6 +1087,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="6ac90070-c7bb-46a5-80a9-4cc49ad71337">
@@ -1108,15 +1111,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1369,6 +1363,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8320F30-E573-4818-9317-DE277DA79035}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5C34FB-9508-4CCC-91FE-4064A913EE20}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1381,14 +1383,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="6ac90070-c7bb-46a5-80a9-4cc49ad71337"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8320F30-E573-4818-9317-DE277DA79035}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>